<commit_message>
Updated employment targets in `policy parameters.xlsx`
New categories: acmales, acfemales, maleswithdep, femaleswithdep have been updated.
</commit_message>
<xml_diff>
--- a/input/EL/policy parameters.xlsx
+++ b/input/EL/policy parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPaths_HU\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://essexuniversity-my.sharepoint.com/personal/mv25449_essex_ac_uk/Documents/WorkCEMPA/SimPathsEU/input_EL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB338366-4843-4835-8D77-7D3E3B4ECC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{EB338366-4843-4835-8D77-7D3E3B4ECC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06F5714F-46CA-2243-986E-9CA32EB6445E}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="10" activeTab="12" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="25120" firstSheet="9" activeTab="12" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
@@ -20,12 +20,12 @@
     <sheet name="students" sheetId="9" r:id="rId5"/>
     <sheet name="partnership" sheetId="4" r:id="rId6"/>
     <sheet name="employment_smales" sheetId="5" r:id="rId7"/>
-    <sheet name="employment_acmales" sheetId="11" r:id="rId8"/>
-    <sheet name="employment_sfemales" sheetId="6" r:id="rId9"/>
-    <sheet name="employment_acfemales" sheetId="12" r:id="rId10"/>
-    <sheet name="employment_malewdep" sheetId="13" r:id="rId11"/>
-    <sheet name="employment_femalewdep" sheetId="14" r:id="rId12"/>
-    <sheet name="employment_couples" sheetId="7" r:id="rId13"/>
+    <sheet name="employment_sfemales" sheetId="6" r:id="rId8"/>
+    <sheet name="employment_couples" sheetId="7" r:id="rId9"/>
+    <sheet name="employment_acmales" sheetId="17" r:id="rId10"/>
+    <sheet name="employment_acfemales" sheetId="19" r:id="rId11"/>
+    <sheet name="employment_femalewdep" sheetId="20" r:id="rId12"/>
+    <sheet name="employment_malewdep" sheetId="21" r:id="rId13"/>
     <sheet name="raw data" sheetId="3" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
   <si>
     <t>CAPITAL LIMITS</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>Share</t>
+  </si>
+  <si>
+    <t>empl_share</t>
   </si>
 </sst>
 </file>
@@ -187,7 +190,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,6 +203,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -225,16 +233,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{74B393FE-FCF6-AD47-9FBD-1BF3F2A2EA51}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -552,13 +563,13 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -566,7 +577,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -574,7 +585,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -582,7 +593,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -590,7 +601,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -601,17 +612,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>37</v>
       </c>
@@ -625,133 +636,126 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719E23B6-17C0-41FE-B44A-4A76A9386EAA}">
-  <dimension ref="A1:B15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34053C06-3093-A547-8E2A-7F4AD8B45E7D}">
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="8.83203125" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2010</v>
-      </c>
-      <c r="B2">
-        <v>0.29414899999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="B1" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
         <v>2011</v>
       </c>
-      <c r="B3">
-        <v>0.29414899999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="B2" s="3">
+        <v>0.34265848994255066</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
         <v>2012</v>
       </c>
-      <c r="B4">
-        <v>0.27185799999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="B3" s="3">
+        <v>0.3118470311164856</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
         <v>2013</v>
       </c>
-      <c r="B5">
-        <v>0.24763199999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="B4" s="3">
+        <v>0.25509169697761536</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
         <v>2014</v>
       </c>
-      <c r="B6">
-        <v>0.22253700000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="B5" s="3">
+        <v>0.26355591416358948</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
         <v>2015</v>
       </c>
-      <c r="B7">
-        <v>0.22546099999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="B6" s="3">
+        <v>0.2731875479221344</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
         <v>2016</v>
       </c>
-      <c r="B8">
-        <v>0.24279899999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="B7" s="3">
+        <v>0.27456456422805786</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
         <v>2017</v>
       </c>
-      <c r="B9">
-        <v>0.24468000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="B8" s="3">
+        <v>0.30087307095527649</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
         <v>2018</v>
       </c>
-      <c r="B10">
-        <v>0.27390300000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="B9" s="3">
+        <v>0.32435283064842224</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
         <v>2019</v>
       </c>
-      <c r="B11">
-        <v>0.313029</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="B10" s="3">
+        <v>0.34818378090858459</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
         <v>2020</v>
       </c>
-      <c r="B12">
-        <v>0.28016600000000003</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="B11" s="3">
+        <v>0.26850566267967224</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
         <v>2021</v>
       </c>
-      <c r="B13">
-        <v>0.27554800000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="B12" s="3">
+        <v>0.31309670209884644</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
         <v>2022</v>
       </c>
-      <c r="B14">
-        <v>0.33879599999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="B13" s="3">
+        <v>0.36759886145591736</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
         <v>2023</v>
       </c>
-      <c r="B15">
-        <v>0.32312099999999999</v>
+      <c r="B14" s="3">
+        <v>0.38148543238639832</v>
       </c>
     </row>
   </sheetData>
@@ -760,133 +764,126 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BD0D06F-6CE1-480E-87E4-F9EE133EFC46}">
-  <dimension ref="A1:B15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA9AC26-AB48-2D4E-9098-57D2685FEAB3}">
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="8.83203125" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2010</v>
-      </c>
-      <c r="B2">
-        <v>0.84780199999999994</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="B1" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
         <v>2011</v>
       </c>
-      <c r="B3">
-        <v>0.84780199999999994</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="B2" s="3">
+        <v>0.29403841495513916</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
         <v>2012</v>
       </c>
-      <c r="B4">
-        <v>0.80887100000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="B3" s="3">
+        <v>0.27003580331802368</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
         <v>2013</v>
       </c>
-      <c r="B5">
-        <v>0.77573499999999995</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="B4" s="3">
+        <v>0.25150370597839355</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
         <v>2014</v>
       </c>
-      <c r="B6">
-        <v>0.75251699999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="B5" s="3">
+        <v>0.22304441034793854</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
         <v>2015</v>
       </c>
-      <c r="B7">
-        <v>0.75262899999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="B6" s="3">
+        <v>0.22579196095466614</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
         <v>2016</v>
       </c>
-      <c r="B8">
-        <v>0.75889499999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="B7" s="3">
+        <v>0.24308605492115021</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
         <v>2017</v>
       </c>
-      <c r="B9">
-        <v>0.79421600000000003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="B8" s="3">
+        <v>0.24757964909076691</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
         <v>2018</v>
       </c>
-      <c r="B10">
-        <v>0.78493500000000005</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="B9" s="3">
+        <v>0.27363336086273193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
         <v>2019</v>
       </c>
-      <c r="B11">
-        <v>0.83127399999999996</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="B10" s="3">
+        <v>0.31426092982292175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
         <v>2020</v>
       </c>
-      <c r="B12">
-        <v>0.88571599999999995</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="B11" s="3">
+        <v>0.27374103665351868</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
         <v>2021</v>
       </c>
-      <c r="B13">
-        <v>0.84921800000000003</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="B12" s="3">
+        <v>0.27762344479560852</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
         <v>2022</v>
       </c>
-      <c r="B14">
-        <v>0.89088400000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="B13" s="3">
+        <v>0.33840039372444153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
         <v>2023</v>
       </c>
-      <c r="B15">
-        <v>0.78691500000000003</v>
+      <c r="B14" s="3">
+        <v>0.32362779974937439</v>
       </c>
     </row>
   </sheetData>
@@ -895,133 +892,126 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FEE925A-70BC-492E-9A66-C8ADBC285DD8}">
-  <dimension ref="A1:B15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E3B675-003C-A042-BB0A-0AFE07D63C97}">
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="8.83203125" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2010</v>
-      </c>
-      <c r="B2">
-        <v>0.26522800000000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="B1" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
         <v>2011</v>
       </c>
-      <c r="B3">
-        <v>0.26522800000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="B2" s="3">
+        <v>0.25936141610145569</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
         <v>2012</v>
       </c>
-      <c r="B4">
-        <v>0.27356799999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="B3" s="3">
+        <v>0.26566678285598755</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
         <v>2013</v>
       </c>
-      <c r="B5">
-        <v>0.273926</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="B4" s="3">
+        <v>0.26629340648651123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
         <v>2014</v>
       </c>
-      <c r="B6">
-        <v>0.23652200000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="B5" s="3">
+        <v>0.23608849942684174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
         <v>2015</v>
       </c>
-      <c r="B7">
-        <v>0.25017800000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="B6" s="3">
+        <v>0.2465636283159256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
         <v>2016</v>
       </c>
-      <c r="B8">
-        <v>0.24973799999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="B7" s="3">
+        <v>0.247969850897789</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
         <v>2017</v>
       </c>
-      <c r="B9">
-        <v>0.26674399999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="B8" s="3">
+        <v>0.26370355486869812</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
         <v>2018</v>
       </c>
-      <c r="B10">
-        <v>0.27819100000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="B9" s="3">
+        <v>0.27386820316314697</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
         <v>2019</v>
       </c>
-      <c r="B11">
-        <v>0.29665599999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="B10" s="3">
+        <v>0.29197514057159424</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
         <v>2020</v>
       </c>
-      <c r="B12">
-        <v>0.30199500000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="B11" s="3">
+        <v>0.29566752910614014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
         <v>2021</v>
       </c>
-      <c r="B13">
-        <v>0.32094800000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="B12" s="3">
+        <v>0.31718915700912476</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
         <v>2022</v>
       </c>
-      <c r="B14">
-        <v>0.34444900000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="B13" s="3">
+        <v>0.3379778265953064</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
         <v>2023</v>
       </c>
-      <c r="B15">
-        <v>0.37901499999999999</v>
+      <c r="B14" s="3">
+        <v>0.3702024519443512</v>
       </c>
     </row>
   </sheetData>
@@ -1030,133 +1020,128 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D244153-91CD-4DE3-A3BE-886BB7506357}">
-  <dimension ref="A1:B15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F62636-5E07-6340-9270-054FA9C7EF00}">
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="L58" sqref="L58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="8.83203125" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2010</v>
-      </c>
-      <c r="B2">
-        <v>0.92523500000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="B1" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
         <v>2011</v>
       </c>
-      <c r="B3">
-        <v>0.92523500000000003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="B2" s="3">
+        <v>0.85731029510498047</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
         <v>2012</v>
       </c>
-      <c r="B4">
-        <v>0.90744100000000005</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="B3" s="3">
+        <v>0.81792652606964111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
         <v>2013</v>
       </c>
-      <c r="B5">
-        <v>0.88748300000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="B4" s="3">
+        <v>0.78032886981964111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
         <v>2014</v>
       </c>
-      <c r="B6">
-        <v>0.89144000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="B5" s="3">
+        <v>0.75630474090576172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
         <v>2015</v>
       </c>
-      <c r="B7">
-        <v>0.91203199999999995</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="B6" s="3">
+        <v>0.75422877073287964</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
         <v>2016</v>
       </c>
-      <c r="B8">
-        <v>0.91222300000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="B7" s="3">
+        <v>0.75874698162078857</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
         <v>2017</v>
       </c>
-      <c r="B9">
-        <v>0.92773099999999997</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="B8" s="3">
+        <v>0.79526036977767944</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
         <v>2018</v>
       </c>
-      <c r="B10">
-        <v>0.92655100000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="B9" s="3">
+        <v>0.78752559423446655</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
         <v>2019</v>
       </c>
-      <c r="B11">
-        <v>0.94273300000000004</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="B10" s="3">
+        <v>0.83185678720474243</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
         <v>2020</v>
       </c>
-      <c r="B12">
-        <v>0.93638600000000005</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="B11" s="3">
+        <v>0.88631808757781982</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
         <v>2021</v>
       </c>
-      <c r="B13">
-        <v>0.93873399999999996</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="B12" s="3">
+        <v>0.85766446590423584</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
         <v>2022</v>
       </c>
-      <c r="B14">
-        <v>0.95450699999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="B13" s="3">
+        <v>0.89023655652999878</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
         <v>2023</v>
       </c>
-      <c r="B15">
-        <v>0.958484</v>
+      <c r="B14" s="3">
+        <v>0.83814162015914917</v>
       </c>
     </row>
   </sheetData>
@@ -1172,9 +1157,9 @@
       <selection activeCell="Y4" sqref="Y4:Y33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>34</v>
       </c>
@@ -1185,7 +1170,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -1201,7 +1186,7 @@
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -1257,7 +1242,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2015</v>
       </c>
@@ -1335,7 +1320,7 @@
         <v>0.6613654059472992</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2016</v>
       </c>
@@ -1414,7 +1399,7 @@
         <v>0.65666662435166534</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2017</v>
       </c>
@@ -1493,7 +1478,7 @@
         <v>0.65162882226991414</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -1572,7 +1557,7 @@
         <v>0.64942413470967808</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2019</v>
       </c>
@@ -1651,7 +1636,7 @@
         <v>0.64547705146902756</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2020</v>
       </c>
@@ -1730,7 +1715,7 @@
         <v>0.64460168570888343</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2021</v>
       </c>
@@ -1809,7 +1794,7 @@
         <v>0.64477324955863657</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2022</v>
       </c>
@@ -1888,7 +1873,7 @@
         <v>0.64570195231543648</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2023</v>
       </c>
@@ -1967,7 +1952,7 @@
         <v>0.64737782355652385</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2024</v>
       </c>
@@ -2028,7 +2013,7 @@
         <v>0.64448143654604106</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2025</v>
       </c>
@@ -2089,7 +2074,7 @@
         <v>0.64389807700679014</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2026</v>
       </c>
@@ -2150,7 +2135,7 @@
         <v>0.63601678163112885</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2027</v>
       </c>
@@ -2211,7 +2196,7 @@
         <v>0.63885715724636716</v>
       </c>
     </row>
-    <row r="17" spans="23:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="23:25" x14ac:dyDescent="0.2">
       <c r="W17">
         <f t="shared" si="11"/>
         <v>2007</v>
@@ -2224,7 +2209,7 @@
         <v>0.63970331929393809</v>
       </c>
     </row>
-    <row r="18" spans="23:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="23:25" x14ac:dyDescent="0.2">
       <c r="W18">
         <f t="shared" si="11"/>
         <v>2008</v>
@@ -2237,7 +2222,7 @@
         <v>0.63745385907812036</v>
       </c>
     </row>
-    <row r="19" spans="23:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="23:25" x14ac:dyDescent="0.2">
       <c r="W19">
         <f t="shared" si="11"/>
         <v>2009</v>
@@ -2250,7 +2235,7 @@
         <v>0.64638142900294271</v>
       </c>
     </row>
-    <row r="20" spans="23:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="23:25" x14ac:dyDescent="0.2">
       <c r="W20">
         <f t="shared" si="11"/>
         <v>2010</v>
@@ -2263,7 +2248,7 @@
         <v>0.64291910814000863</v>
       </c>
     </row>
-    <row r="21" spans="23:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="23:25" x14ac:dyDescent="0.2">
       <c r="W21">
         <f t="shared" si="11"/>
         <v>2011</v>
@@ -2276,7 +2261,7 @@
         <v>0.64183543445918845</v>
       </c>
     </row>
-    <row r="22" spans="23:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="23:25" x14ac:dyDescent="0.2">
       <c r="W22">
         <f t="shared" si="11"/>
         <v>2012</v>
@@ -2289,7 +2274,7 @@
         <v>0.64457311813040019</v>
       </c>
     </row>
-    <row r="23" spans="23:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="23:25" x14ac:dyDescent="0.2">
       <c r="W23">
         <f t="shared" si="11"/>
         <v>2013</v>
@@ -2302,7 +2287,7 @@
         <v>0.64501821298769013</v>
       </c>
     </row>
-    <row r="24" spans="23:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="23:25" x14ac:dyDescent="0.2">
       <c r="W24">
         <f t="shared" si="11"/>
         <v>2014</v>
@@ -2315,7 +2300,7 @@
         <v>0.64303300577959377</v>
       </c>
     </row>
-    <row r="25" spans="23:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="23:25" x14ac:dyDescent="0.2">
       <c r="W25">
         <f t="shared" si="11"/>
         <v>2015</v>
@@ -2328,7 +2313,7 @@
         <v>0.64350137796521267</v>
       </c>
     </row>
-    <row r="26" spans="23:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="23:25" x14ac:dyDescent="0.2">
       <c r="W26">
         <f t="shared" si="11"/>
         <v>2016</v>
@@ -2341,7 +2326,7 @@
         <v>0.64443090532156433</v>
       </c>
     </row>
-    <row r="27" spans="23:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="23:25" x14ac:dyDescent="0.2">
       <c r="W27">
         <f t="shared" si="11"/>
         <v>2017</v>
@@ -2354,7 +2339,7 @@
         <v>0.64369538754708922</v>
       </c>
     </row>
-    <row r="28" spans="23:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="23:25" x14ac:dyDescent="0.2">
       <c r="W28">
         <f t="shared" si="11"/>
         <v>2018</v>
@@ -2367,7 +2352,7 @@
         <v>0.64389678969687036</v>
       </c>
     </row>
-    <row r="29" spans="23:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="23:25" x14ac:dyDescent="0.2">
       <c r="W29">
         <f t="shared" si="11"/>
         <v>2019</v>
@@ -2380,7 +2365,7 @@
         <v>0.63975244582712099</v>
       </c>
     </row>
-    <row r="30" spans="23:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="23:25" x14ac:dyDescent="0.2">
       <c r="W30">
         <f t="shared" si="11"/>
         <v>2020</v>
@@ -2393,7 +2378,7 @@
         <v>0.64948824720523413</v>
       </c>
     </row>
-    <row r="31" spans="23:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="23:25" x14ac:dyDescent="0.2">
       <c r="W31">
         <f t="shared" si="11"/>
         <v>2021</v>
@@ -2406,7 +2391,7 @@
         <v>0.64443733677754689</v>
       </c>
     </row>
-    <row r="32" spans="23:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="23:25" x14ac:dyDescent="0.2">
       <c r="W32">
         <v>2022</v>
       </c>
@@ -2415,7 +2400,7 @@
         <v>0.64425404141077236</v>
       </c>
     </row>
-    <row r="33" spans="23:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="23:25" x14ac:dyDescent="0.2">
       <c r="W33">
         <v>2023</v>
       </c>
@@ -2435,9 +2420,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -2445,7 +2430,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2010</v>
       </c>
@@ -2453,7 +2438,7 @@
         <v>9.3950000000000006E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2011</v>
       </c>
@@ -2461,7 +2446,7 @@
         <v>9.3950000000000006E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2012</v>
       </c>
@@ -2469,7 +2454,7 @@
         <v>7.3379999999999999E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2013</v>
       </c>
@@ -2477,7 +2462,7 @@
         <v>7.3130000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2014</v>
       </c>
@@ -2485,7 +2470,7 @@
         <v>8.2740000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2015</v>
       </c>
@@ -2493,7 +2478,7 @@
         <v>9.613E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2016</v>
       </c>
@@ -2501,7 +2486,7 @@
         <v>1.0828000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2017</v>
       </c>
@@ -2509,7 +2494,7 @@
         <v>1.192E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2018</v>
       </c>
@@ -2517,7 +2502,7 @@
         <v>1.3712999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2019</v>
       </c>
@@ -2525,7 +2510,7 @@
         <v>1.6736000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2020</v>
       </c>
@@ -2533,7 +2518,7 @@
         <v>1.6816000000000001E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2021</v>
       </c>
@@ -2541,7 +2526,7 @@
         <v>6.842E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2022</v>
       </c>
@@ -2549,7 +2534,7 @@
         <v>8.2850000000000007E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2023</v>
       </c>
@@ -2568,9 +2553,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -2599,7 +2584,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2015</v>
       </c>
@@ -2628,7 +2613,7 @@
         <v>23250</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2016</v>
       </c>
@@ -2657,7 +2642,7 @@
         <v>23088.381330685203</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2017</v>
       </c>
@@ -2687,7 +2672,7 @@
       </c>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2018</v>
       </c>
@@ -2717,7 +2702,7 @@
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2019</v>
       </c>
@@ -2747,7 +2732,7 @@
       </c>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2020</v>
       </c>
@@ -2777,7 +2762,7 @@
       </c>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2021</v>
       </c>
@@ -2807,7 +2792,7 @@
       </c>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2022</v>
       </c>
@@ -2837,7 +2822,7 @@
       </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2023</v>
       </c>
@@ -2867,7 +2852,7 @@
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2024</v>
       </c>
@@ -2897,7 +2882,7 @@
       </c>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2025</v>
       </c>
@@ -2927,7 +2912,7 @@
       </c>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2026</v>
       </c>
@@ -2957,7 +2942,7 @@
       </c>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2027</v>
       </c>
@@ -2987,10 +2972,10 @@
       </c>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K16" s="1"/>
     </row>
   </sheetData>
@@ -3004,9 +2989,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -3014,7 +2999,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2010</v>
       </c>
@@ -3022,7 +3007,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2011</v>
       </c>
@@ -3030,7 +3015,7 @@
         <v>0.20200000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2012</v>
       </c>
@@ -3038,7 +3023,7 @@
         <v>0.20300000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2013</v>
       </c>
@@ -3046,7 +3031,7 @@
         <v>0.20599999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2014</v>
       </c>
@@ -3054,7 +3039,7 @@
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2015</v>
       </c>
@@ -3062,7 +3047,7 @@
         <v>0.215</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2016</v>
       </c>
@@ -3070,7 +3055,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2017</v>
       </c>
@@ -3078,7 +3063,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2018</v>
       </c>
@@ -3086,7 +3071,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2019</v>
       </c>
@@ -3094,7 +3079,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2020</v>
       </c>
@@ -3102,7 +3087,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2021</v>
       </c>
@@ -3110,7 +3095,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2022</v>
       </c>
@@ -3118,7 +3103,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2023</v>
       </c>
@@ -3139,9 +3124,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -3149,7 +3134,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2010</v>
       </c>
@@ -3157,7 +3142,7 @@
         <v>0.23899999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2011</v>
       </c>
@@ -3165,7 +3150,7 @@
         <v>0.23899999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2012</v>
       </c>
@@ -3173,7 +3158,7 @@
         <v>0.23400000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2013</v>
       </c>
@@ -3181,7 +3166,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2014</v>
       </c>
@@ -3189,7 +3174,7 @@
         <v>0.22600000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2015</v>
       </c>
@@ -3197,7 +3182,7 @@
         <v>0.219</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2016</v>
       </c>
@@ -3205,7 +3190,7 @@
         <v>0.218</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2017</v>
       </c>
@@ -3213,7 +3198,7 @@
         <v>0.21299999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2018</v>
       </c>
@@ -3221,7 +3206,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2019</v>
       </c>
@@ -3229,7 +3214,7 @@
         <v>0.20499999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2020</v>
       </c>
@@ -3237,7 +3222,7 @@
         <v>0.20399999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2021</v>
       </c>
@@ -3245,7 +3230,7 @@
         <v>0.19700000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2022</v>
       </c>
@@ -3253,7 +3238,7 @@
         <v>0.19500000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2023</v>
       </c>
@@ -3261,7 +3246,7 @@
         <v>0.188</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2024</v>
       </c>
@@ -3269,7 +3254,7 @@
         <v>0.188</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2025</v>
       </c>
@@ -3277,7 +3262,7 @@
         <v>0.188</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2026</v>
       </c>
@@ -3285,7 +3270,7 @@
         <v>0.188</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2027</v>
       </c>
@@ -3293,7 +3278,7 @@
         <v>0.188</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2028</v>
       </c>
@@ -3301,7 +3286,7 @@
         <v>0.188</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2029</v>
       </c>
@@ -3309,7 +3294,7 @@
         <v>0.188</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2030</v>
       </c>
@@ -3317,7 +3302,7 @@
         <v>0.188</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2031</v>
       </c>
@@ -3325,7 +3310,7 @@
         <v>0.188</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2032</v>
       </c>
@@ -3333,7 +3318,7 @@
         <v>0.188</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2033</v>
       </c>
@@ -3341,7 +3326,7 @@
         <v>0.188</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2034</v>
       </c>
@@ -3349,7 +3334,7 @@
         <v>0.188</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2035</v>
       </c>
@@ -3370,9 +3355,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -3380,7 +3365,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2010</v>
       </c>
@@ -3388,7 +3373,7 @@
         <v>0.64039999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2011</v>
       </c>
@@ -3396,7 +3381,7 @@
         <v>0.64039999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2012</v>
       </c>
@@ -3404,7 +3389,7 @@
         <v>0.63329999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2013</v>
       </c>
@@ -3412,7 +3397,7 @@
         <v>0.623</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2014</v>
       </c>
@@ -3420,7 +3405,7 @@
         <v>0.62119999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2015</v>
       </c>
@@ -3428,7 +3413,7 @@
         <v>0.6179</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2016</v>
       </c>
@@ -3436,7 +3421,7 @@
         <v>0.61819999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2017</v>
       </c>
@@ -3444,7 +3429,7 @@
         <v>0.6129</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2018</v>
       </c>
@@ -3452,7 +3437,7 @@
         <v>0.61429999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2019</v>
       </c>
@@ -3460,7 +3445,7 @@
         <v>0.61729999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2020</v>
       </c>
@@ -3468,7 +3453,7 @@
         <v>0.61029999999999995</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2021</v>
       </c>
@@ -3476,7 +3461,7 @@
         <v>0.61780000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2022</v>
       </c>
@@ -3484,7 +3469,7 @@
         <v>0.61570000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2023</v>
       </c>
@@ -3492,7 +3477,7 @@
         <v>0.61009999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2024</v>
       </c>
@@ -3500,7 +3485,7 @@
         <v>0.61009999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2025</v>
       </c>
@@ -3508,7 +3493,7 @@
         <v>0.61009999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2026</v>
       </c>
@@ -3516,7 +3501,7 @@
         <v>0.61009999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2027</v>
       </c>
@@ -3524,7 +3509,7 @@
         <v>0.61009999999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2028</v>
       </c>
@@ -3532,7 +3517,7 @@
         <v>0.61009999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2029</v>
       </c>
@@ -3540,7 +3525,7 @@
         <v>0.61009999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2030</v>
       </c>
@@ -3548,7 +3533,7 @@
         <v>0.61009999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2031</v>
       </c>
@@ -3556,7 +3541,7 @@
         <v>0.61009999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2032</v>
       </c>
@@ -3564,7 +3549,7 @@
         <v>0.61009999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2033</v>
       </c>
@@ -3572,7 +3557,7 @@
         <v>0.61009999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2034</v>
       </c>
@@ -3580,7 +3565,7 @@
         <v>0.61009999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2035</v>
       </c>
@@ -3602,9 +3587,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -3612,7 +3597,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2010</v>
       </c>
@@ -3620,7 +3605,7 @@
         <v>0.70775399999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2011</v>
       </c>
@@ -3628,7 +3613,7 @@
         <v>0.70775399999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2012</v>
       </c>
@@ -3636,7 +3621,7 @@
         <v>0.68374000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2013</v>
       </c>
@@ -3644,7 +3629,7 @@
         <v>0.64686200000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2014</v>
       </c>
@@ -3652,7 +3637,7 @@
         <v>0.64708299999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2015</v>
       </c>
@@ -3660,7 +3645,7 @@
         <v>0.64515100000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2016</v>
       </c>
@@ -3668,7 +3653,7 @@
         <v>0.66195099999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2017</v>
       </c>
@@ -3676,7 +3661,7 @@
         <v>0.67321299999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2018</v>
       </c>
@@ -3684,7 +3669,7 @@
         <v>0.68717399999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2019</v>
       </c>
@@ -3692,7 +3677,7 @@
         <v>0.698577</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2020</v>
       </c>
@@ -3700,7 +3685,7 @@
         <v>0.705511</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2021</v>
       </c>
@@ -3708,7 +3693,7 @@
         <v>0.72767700000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2022</v>
       </c>
@@ -3716,7 +3701,7 @@
         <v>0.74404400000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2023</v>
       </c>
@@ -3730,141 +3715,6 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D7884F4-8D94-407C-9CEB-CF990A77FD4A}">
-  <dimension ref="A1:B15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2010</v>
-      </c>
-      <c r="B2">
-        <v>0.349132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2011</v>
-      </c>
-      <c r="B3">
-        <v>0.349132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2012</v>
-      </c>
-      <c r="B4">
-        <v>0.349132</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2013</v>
-      </c>
-      <c r="B5">
-        <v>0.30974299999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2014</v>
-      </c>
-      <c r="B6">
-        <v>0.25676199999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2015</v>
-      </c>
-      <c r="B7">
-        <v>0.26411699999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2016</v>
-      </c>
-      <c r="B8">
-        <v>0.27359499999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2017</v>
-      </c>
-      <c r="B9">
-        <v>0.27618300000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2018</v>
-      </c>
-      <c r="B10">
-        <v>0.30072199999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2019</v>
-      </c>
-      <c r="B11">
-        <v>0.32430500000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2020</v>
-      </c>
-      <c r="B12">
-        <v>0.351267</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>2021</v>
-      </c>
-      <c r="B13">
-        <v>0.26828200000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>2022</v>
-      </c>
-      <c r="B14">
-        <v>0.31243900000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>2023</v>
-      </c>
-      <c r="B15">
-        <v>0.36913600000000002</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ADCB18-5B9A-4019-89E5-BA38EA9BE54A}">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -3872,9 +3722,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -3882,7 +3732,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2010</v>
       </c>
@@ -3890,7 +3740,7 @@
         <v>0.34815200000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2011</v>
       </c>
@@ -3898,7 +3748,7 @@
         <v>0.34815200000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2012</v>
       </c>
@@ -3906,7 +3756,7 @@
         <v>0.38269999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2013</v>
       </c>
@@ -3914,7 +3764,7 @@
         <v>0.35855999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2014</v>
       </c>
@@ -3922,7 +3772,7 @@
         <v>0.34620200000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2015</v>
       </c>
@@ -3930,7 +3780,7 @@
         <v>0.36657099999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2016</v>
       </c>
@@ -3938,7 +3788,7 @@
         <v>0.36750899999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2017</v>
       </c>
@@ -3946,7 +3796,7 @@
         <v>0.36946400000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2018</v>
       </c>
@@ -3954,7 +3804,7 @@
         <v>0.36212800000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2019</v>
       </c>
@@ -3962,7 +3812,7 @@
         <v>0.35998599999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2020</v>
       </c>
@@ -3970,7 +3820,7 @@
         <v>0.347271</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2021</v>
       </c>
@@ -3978,7 +3828,7 @@
         <v>0.38936500000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2022</v>
       </c>
@@ -3986,12 +3836,147 @@
         <v>0.39210400000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2023</v>
       </c>
       <c r="B15">
         <v>0.40636100000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D244153-91CD-4DE3-A3BE-886BB7506357}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2010</v>
+      </c>
+      <c r="B2">
+        <v>0.92523500000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2011</v>
+      </c>
+      <c r="B3">
+        <v>0.92523500000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2012</v>
+      </c>
+      <c r="B4">
+        <v>0.90744100000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2013</v>
+      </c>
+      <c r="B5">
+        <v>0.88748300000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2014</v>
+      </c>
+      <c r="B6">
+        <v>0.89144000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2015</v>
+      </c>
+      <c r="B7">
+        <v>0.91203199999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2016</v>
+      </c>
+      <c r="B8">
+        <v>0.91222300000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2017</v>
+      </c>
+      <c r="B9">
+        <v>0.92773099999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2018</v>
+      </c>
+      <c r="B10">
+        <v>0.92655100000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2019</v>
+      </c>
+      <c r="B11">
+        <v>0.94273300000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2020</v>
+      </c>
+      <c r="B12">
+        <v>0.93638600000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2021</v>
+      </c>
+      <c r="B13">
+        <v>0.93873399999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2022</v>
+      </c>
+      <c r="B14">
+        <v>0.95450699999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2023</v>
+      </c>
+      <c r="B15">
+        <v>0.958484</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update AdultChildFlag definition and corrected PSA; added RootSearch2 a corrected exit condition -PSA is now country and gender dependent - AdultChild flag is defined for adults who live with parents who are below psa and are not retired. - RootSearch2 with a corrected exit and improved accuracy (tol) conditions is applied in employment alignment.
</commit_message>
<xml_diff>
--- a/input/EL/policy parameters.xlsx
+++ b/input/EL/policy parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://essexuniversity-my.sharepoint.com/personal/mv25449_essex_ac_uk/Documents/WorkCEMPA/SimPathsEU/input_EL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pineapple/IdeaProjects/SimPathsEUmerged/input/EL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{EB338366-4843-4835-8D77-7D3E3B4ECC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06F5714F-46CA-2243-986E-9CA32EB6445E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9853DF00-832E-1D49-A411-0405D0901C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="25120" firstSheet="9" activeTab="12" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="25120" firstSheet="6" activeTab="6" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
   <si>
     <t>CAPITAL LIMITS</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t>MINIMUM INCOME GUARANTEE PER WEEK</t>
-  </si>
-  <si>
-    <t>employed_share</t>
   </si>
   <si>
     <t>26/08/2024 (JV)</t>
@@ -190,7 +187,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +205,12 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -237,11 +240,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,7 +602,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -624,10 +628,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
         <v>37</v>
-      </c>
-      <c r="C9" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -639,7 +643,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34053C06-3093-A547-8E2A-7F4AD8B45E7D}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -647,115 +653,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>43</v>
+      <c r="B1" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+      <c r="A2" s="4">
         <v>2011</v>
       </c>
-      <c r="B2" s="3">
-        <v>0.34265848994255066</v>
+      <c r="B2" s="4">
+        <v>0.351192</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="A3" s="4">
         <v>2012</v>
       </c>
-      <c r="B3" s="3">
-        <v>0.3118470311164856</v>
+      <c r="B3" s="4">
+        <v>0.31094899999999998</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4" s="4">
         <v>2013</v>
       </c>
-      <c r="B4" s="3">
-        <v>0.25509169697761536</v>
+      <c r="B4" s="4">
+        <v>0.25732899999999997</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="A5" s="4">
         <v>2014</v>
       </c>
-      <c r="B5" s="3">
-        <v>0.26355591416358948</v>
+      <c r="B5" s="4">
+        <v>0.26499600000000001</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="A6" s="4">
         <v>2015</v>
       </c>
-      <c r="B6" s="3">
-        <v>0.2731875479221344</v>
+      <c r="B6" s="4">
+        <v>0.27389400000000003</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+      <c r="A7" s="4">
         <v>2016</v>
       </c>
-      <c r="B7" s="3">
-        <v>0.27456456422805786</v>
+      <c r="B7" s="4">
+        <v>0.27547300000000002</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+      <c r="A8" s="4">
         <v>2017</v>
       </c>
-      <c r="B8" s="3">
-        <v>0.30087307095527649</v>
+      <c r="B8" s="4">
+        <v>0.30065700000000001</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+      <c r="A9" s="4">
         <v>2018</v>
       </c>
-      <c r="B9" s="3">
-        <v>0.32435283064842224</v>
+      <c r="B9" s="4">
+        <v>0.324797</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+      <c r="A10" s="4">
         <v>2019</v>
       </c>
-      <c r="B10" s="3">
-        <v>0.34818378090858459</v>
+      <c r="B10" s="4">
+        <v>0.35145100000000001</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+      <c r="A11" s="4">
         <v>2020</v>
       </c>
-      <c r="B11" s="3">
-        <v>0.26850566267967224</v>
+      <c r="B11" s="4">
+        <v>0.26827400000000001</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+      <c r="A12" s="4">
         <v>2021</v>
       </c>
-      <c r="B12" s="3">
-        <v>0.31309670209884644</v>
+      <c r="B12" s="4">
+        <v>0.31126100000000001</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+      <c r="A13" s="4">
         <v>2022</v>
       </c>
-      <c r="B13" s="3">
-        <v>0.36759886145591736</v>
+      <c r="B13" s="4">
+        <v>0.367871</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+      <c r="A14" s="4">
         <v>2023</v>
       </c>
-      <c r="B14" s="3">
-        <v>0.38148543238639832</v>
+      <c r="B14" s="4">
+        <v>0.38261000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -767,7 +773,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA9AC26-AB48-2D4E-9098-57D2685FEAB3}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -775,115 +783,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>43</v>
+      <c r="B1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+      <c r="A2">
         <v>2011</v>
       </c>
-      <c r="B2" s="3">
-        <v>0.29403841495513916</v>
+      <c r="B2">
+        <v>0.29207861423492432</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="A3">
         <v>2012</v>
       </c>
-      <c r="B3" s="3">
-        <v>0.27003580331802368</v>
+      <c r="B3">
+        <v>0.27055910229682922</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4">
         <v>2013</v>
       </c>
-      <c r="B4" s="3">
-        <v>0.25150370597839355</v>
+      <c r="B4">
+        <v>0.24703994393348694</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="A5">
         <v>2014</v>
       </c>
-      <c r="B5" s="3">
-        <v>0.22304441034793854</v>
+      <c r="B5">
+        <v>0.22169908881187439</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="A6">
         <v>2015</v>
       </c>
-      <c r="B6" s="3">
-        <v>0.22579196095466614</v>
+      <c r="B6">
+        <v>0.22514611482620239</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+      <c r="A7">
         <v>2016</v>
       </c>
-      <c r="B7" s="3">
-        <v>0.24308605492115021</v>
+      <c r="B7">
+        <v>0.24366115033626556</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+      <c r="A8">
         <v>2017</v>
       </c>
-      <c r="B8" s="3">
-        <v>0.24757964909076691</v>
+      <c r="B8">
+        <v>0.24503222107887268</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+      <c r="A9">
         <v>2018</v>
       </c>
-      <c r="B9" s="3">
-        <v>0.27363336086273193</v>
+      <c r="B9">
+        <v>0.27350795269012451</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+      <c r="A10">
         <v>2019</v>
       </c>
-      <c r="B10" s="3">
-        <v>0.31426092982292175</v>
+      <c r="B10">
+        <v>0.31282317638397217</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+      <c r="A11">
         <v>2020</v>
       </c>
-      <c r="B11" s="3">
-        <v>0.27374103665351868</v>
+      <c r="B11">
+        <v>0.27996817231178284</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+      <c r="A12">
         <v>2021</v>
       </c>
-      <c r="B12" s="3">
-        <v>0.27762344479560852</v>
+      <c r="B12">
+        <v>0.27696380019187927</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+      <c r="A13">
         <v>2022</v>
       </c>
-      <c r="B13" s="3">
-        <v>0.33840039372444153</v>
+      <c r="B13">
+        <v>0.34032073616981506</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+      <c r="A14">
         <v>2023</v>
       </c>
-      <c r="B14" s="3">
-        <v>0.32362779974937439</v>
+      <c r="B14">
+        <v>0.32536032795906067</v>
       </c>
     </row>
   </sheetData>
@@ -895,7 +903,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E3B675-003C-A042-BB0A-0AFE07D63C97}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -903,115 +913,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>43</v>
+      <c r="B1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+      <c r="A2">
         <v>2011</v>
       </c>
-      <c r="B2" s="3">
-        <v>0.25936141610145569</v>
+      <c r="B2">
+        <v>0.26944726705551147</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="A3">
         <v>2012</v>
       </c>
-      <c r="B3" s="3">
-        <v>0.26566678285598755</v>
+      <c r="B3">
+        <v>0.28485673666000366</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4">
         <v>2013</v>
       </c>
-      <c r="B4" s="3">
-        <v>0.26629340648651123</v>
+      <c r="B4">
+        <v>0.28213942050933838</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="A5">
         <v>2014</v>
       </c>
-      <c r="B5" s="3">
-        <v>0.23608849942684174</v>
+      <c r="B5">
+        <v>0.24857573211193085</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="A6">
         <v>2015</v>
       </c>
-      <c r="B6" s="3">
-        <v>0.2465636283159256</v>
+      <c r="B6">
+        <v>0.26086214184761047</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+      <c r="A7">
         <v>2016</v>
       </c>
-      <c r="B7" s="3">
-        <v>0.247969850897789</v>
+      <c r="B7">
+        <v>0.2633550763130188</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+      <c r="A8">
         <v>2017</v>
       </c>
-      <c r="B8" s="3">
-        <v>0.26370355486869812</v>
+      <c r="B8">
+        <v>0.27866613864898682</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+      <c r="A9">
         <v>2018</v>
       </c>
-      <c r="B9" s="3">
-        <v>0.27386820316314697</v>
+      <c r="B9">
+        <v>0.28522393107414246</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+      <c r="A10">
         <v>2019</v>
       </c>
-      <c r="B10" s="3">
-        <v>0.29197514057159424</v>
+      <c r="B10">
+        <v>0.29886516928672791</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+      <c r="A11">
         <v>2020</v>
       </c>
-      <c r="B11" s="3">
-        <v>0.29566752910614014</v>
+      <c r="B11">
+        <v>0.3018018901348114</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+      <c r="A12">
         <v>2021</v>
       </c>
-      <c r="B12" s="3">
-        <v>0.31718915700912476</v>
+      <c r="B12">
+        <v>0.32455584406852722</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+      <c r="A13">
         <v>2022</v>
       </c>
-      <c r="B13" s="3">
-        <v>0.3379778265953064</v>
+      <c r="B13">
+        <v>0.34433570504188538</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+      <c r="A14">
         <v>2023</v>
       </c>
-      <c r="B14" s="3">
-        <v>0.3702024519443512</v>
+      <c r="B14">
+        <v>0.38466408848762512</v>
       </c>
     </row>
   </sheetData>
@@ -1023,8 +1033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F62636-5E07-6340-9270-054FA9C7EF00}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L58" sqref="L58"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1033,115 +1043,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>43</v>
+      <c r="B1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+      <c r="A2">
         <v>2011</v>
       </c>
-      <c r="B2" s="3">
-        <v>0.85731029510498047</v>
+      <c r="B2">
+        <v>0.86429673433303833</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="A3">
         <v>2012</v>
       </c>
-      <c r="B3" s="3">
-        <v>0.81792652606964111</v>
+      <c r="B3">
+        <v>0.79113441705703735</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4">
         <v>2013</v>
       </c>
-      <c r="B4" s="3">
-        <v>0.78032886981964111</v>
+      <c r="B4">
+        <v>0.76833385229110718</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="A5">
         <v>2014</v>
       </c>
-      <c r="B5" s="3">
-        <v>0.75630474090576172</v>
+      <c r="B5">
+        <v>0.73654413223266602</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="A6">
         <v>2015</v>
       </c>
-      <c r="B6" s="3">
-        <v>0.75422877073287964</v>
+      <c r="B6">
+        <v>0.76233726739883423</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+      <c r="A7">
         <v>2016</v>
       </c>
-      <c r="B7" s="3">
-        <v>0.75874698162078857</v>
+      <c r="B7">
+        <v>0.75591021776199341</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+      <c r="A8">
         <v>2017</v>
       </c>
-      <c r="B8" s="3">
-        <v>0.79526036977767944</v>
+      <c r="B8">
+        <v>0.80901944637298584</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+      <c r="A9">
         <v>2018</v>
       </c>
-      <c r="B9" s="3">
-        <v>0.78752559423446655</v>
+      <c r="B9">
+        <v>0.78865730762481689</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+      <c r="A10">
         <v>2019</v>
       </c>
-      <c r="B10" s="3">
-        <v>0.83185678720474243</v>
+      <c r="B10">
+        <v>0.79241859912872314</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+      <c r="A11">
         <v>2020</v>
       </c>
-      <c r="B11" s="3">
-        <v>0.88631808757781982</v>
+      <c r="B11">
+        <v>0.88255161046981812</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+      <c r="A12">
         <v>2021</v>
       </c>
-      <c r="B12" s="3">
-        <v>0.85766446590423584</v>
+      <c r="B12">
+        <v>0.85671079158782959</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+      <c r="A13">
         <v>2022</v>
       </c>
-      <c r="B13" s="3">
-        <v>0.89023655652999878</v>
+      <c r="B13">
+        <v>0.89240550994873047</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+      <c r="A14">
         <v>2023</v>
       </c>
-      <c r="B14" s="3">
-        <v>0.83814162015914917</v>
+      <c r="B14">
+        <v>0.83246976137161255</v>
       </c>
     </row>
   </sheetData>
@@ -1236,10 +1246,10 @@
         <v>31</v>
       </c>
       <c r="X3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y3" t="s">
         <v>39</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
@@ -2424,10 +2434,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
         <v>41</v>
-      </c>
-      <c r="B1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -2993,10 +3003,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
         <v>41</v>
-      </c>
-      <c r="B1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -3128,10 +3138,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
         <v>41</v>
-      </c>
-      <c r="B1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -3359,10 +3369,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
         <v>41</v>
-      </c>
-      <c r="B1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -3581,10 +3591,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C02B2D7-F4EC-4D40-840B-FB6BA99B9F2B}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3594,119 +3604,111 @@
         <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="B2">
-        <v>0.70775399999999999</v>
+        <v>0.52254068851470947</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="B3">
-        <v>0.70775399999999999</v>
+        <v>0.52615827322006226</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="B4">
-        <v>0.68374000000000001</v>
+        <v>0.46906697750091553</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="B5">
-        <v>0.64686200000000005</v>
+        <v>0.47447490692138672</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="B6">
-        <v>0.64708299999999996</v>
+        <v>0.47796085476875305</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B7">
-        <v>0.64515100000000003</v>
+        <v>0.49773642420768738</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B8">
-        <v>0.66195099999999996</v>
+        <v>0.51125496625900269</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B9">
-        <v>0.67321299999999995</v>
+        <v>0.53906542062759399</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B10">
-        <v>0.68717399999999995</v>
+        <v>0.54740816354751587</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="B11">
-        <v>0.698577</v>
+        <v>0.56602108478546143</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B12">
-        <v>0.705511</v>
+        <v>0.58690434694290161</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B13">
-        <v>0.72767700000000002</v>
+        <v>0.60512912273406982</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B14">
-        <v>0.74404400000000004</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>2023</v>
-      </c>
-      <c r="B15">
-        <v>0.75032299999999996</v>
+        <v>0.61477339267730713</v>
       </c>
     </row>
   </sheetData>
@@ -3716,10 +3718,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ADCB18-5B9A-4019-89E5-BA38EA9BE54A}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3729,119 +3731,111 @@
         <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="B2">
-        <v>0.34815200000000002</v>
+        <v>0.21119232475757599</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="B3">
-        <v>0.34815200000000002</v>
+        <v>0.24291148781776428</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="B4">
-        <v>0.38269999999999998</v>
+        <v>0.25585943460464478</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="B5">
-        <v>0.35855999999999999</v>
+        <v>0.2502371072769165</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="B6">
-        <v>0.34620200000000001</v>
+        <v>0.27151688933372498</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B7">
-        <v>0.36657099999999998</v>
+        <v>0.27320361137390137</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B8">
-        <v>0.36750899999999997</v>
+        <v>0.27818933129310608</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B9">
-        <v>0.36946400000000001</v>
+        <v>0.26564255356788635</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B10">
-        <v>0.36212800000000001</v>
+        <v>0.27498957514762878</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="B11">
-        <v>0.35998599999999997</v>
+        <v>0.27618974447250366</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B12">
-        <v>0.347271</v>
+        <v>0.2884819507598877</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B13">
-        <v>0.38936500000000002</v>
+        <v>0.29267486929893494</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B14">
-        <v>0.39210400000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>2023</v>
-      </c>
-      <c r="B15">
-        <v>0.40636100000000003</v>
+        <v>0.31361463665962219</v>
       </c>
     </row>
   </sheetData>
@@ -3851,10 +3845,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D244153-91CD-4DE3-A3BE-886BB7506357}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3864,119 +3858,111 @@
         <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="B2">
-        <v>0.92523500000000003</v>
+        <v>0.93070703744888306</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="B3">
-        <v>0.92523500000000003</v>
+        <v>0.91424030065536499</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="B4">
-        <v>0.90744100000000005</v>
+        <v>0.8914649486541748</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="B5">
-        <v>0.88748300000000002</v>
+        <v>0.89563721418380737</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="B6">
-        <v>0.89144000000000001</v>
+        <v>0.91292649507522583</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B7">
-        <v>0.91203199999999995</v>
+        <v>0.91583895683288574</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B8">
-        <v>0.91222300000000001</v>
+        <v>0.93232297897338867</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B9">
-        <v>0.92773099999999997</v>
+        <v>0.93245691061019897</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B10">
-        <v>0.92655100000000001</v>
+        <v>0.94892263412475586</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="B11">
-        <v>0.94273300000000004</v>
+        <v>0.9398379921913147</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B12">
-        <v>0.93638600000000005</v>
+        <v>0.94484466314315796</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B13">
-        <v>0.93873399999999996</v>
+        <v>0.95866239070892334</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B14">
-        <v>0.95450699999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>2023</v>
-      </c>
-      <c r="B15">
-        <v>0.958484</v>
+        <v>0.96066474914550781</v>
       </c>
     </row>
   </sheetData>

</xml_diff>